<commit_message>
update test executing bash script
</commit_message>
<xml_diff>
--- a/results/preliminary results.xlsx
+++ b/results/preliminary results.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoeKifle/Documents/Joetelila/RemoteProjects/Multi-Thread-KNN/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A7EBF9-25A4-BE4E-AD86-96C189D282CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE4CC38-73A3-9F47-B639-16933D642FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{3294C2D5-AD59-2B4A-A6EC-F78AAA2A5DCB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{3294C2D5-AD59-2B4A-A6EC-F78AAA2A5DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="stl_par_knn" sheetId="2" r:id="rId2"/>
     <sheet name="ff_pfr_knn" sheetId="3" r:id="rId3"/>
     <sheet name="openmp_knn, k = 10, input_mediu" sheetId="4" r:id="rId4"/>
+    <sheet name="STL Seq" sheetId="5" r:id="rId5"/>
+    <sheet name="STL Par" sheetId="6" r:id="rId6"/>
+    <sheet name="FF Par" sheetId="7" r:id="rId7"/>
+    <sheet name="openMP Par" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2874" uniqueCount="335">
   <si>
     <t>Threads</t>
   </si>
@@ -829,6 +833,210 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>[STL CPP Sequential], [input_10k_s100.txt], [10 runs]: 3744877</t>
+  </si>
+  <si>
+    <t>[STL CPP Sequential], [input_50k_s200.txt], [10 runs]: 94805036</t>
+  </si>
+  <si>
+    <t>[STL CPP Sequential], [input_100k_s300.txt], [10 runs]: 372073573</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[1 threads] [10 runs] : 3743759</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[2 threads] [10 runs] : 5645892</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[4 threads] [10 runs] : 6654671</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[8 threads] [10 runs] : 7166189</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[16 threads] [10 runs] : 7494721</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[32 threads] [10 runs] : 7648862</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[64 threads] [10 runs] : 7793584</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[128 threads] [10 runs] : 7942890</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_10k_s100.txt],[256 threads] [10 runs] : 8130937</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[1 threads] [10 runs] : 98202341</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[2 threads] [10 runs] : 147394212</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[4 threads] [10 runs] : 173105621</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[8 threads] [10 runs] : 186037959</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[16 threads] [10 runs] : 192528426</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[32 threads] [10 runs] : 196020961</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[64 threads] [10 runs] : 198341238</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[128 threads] [10 runs] : 200139919</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_50k_s200.txt],[256 threads] [10 runs] : 201454318</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[1 threads] [10 runs] : 376661565</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[2 threads] [10 runs] : 563950061</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[4 threads] [10 runs] : 665061583</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[8 threads] [10 runs] : 715836550</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[16 threads] [10 runs] : 741259864</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[32 threads] [10 runs] : 754119194</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[64 threads] [10 runs] : 761001617</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[128 threads] [10 runs] : 766082799</t>
+  </si>
+  <si>
+    <t>[FF Parallel for] , [input_100k_s300.txt],[256 threads] [10 runs] : 770394690</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[1 threads] [10 runs] : 3757566</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[2 threads] [10 runs] : 5748439</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[4 threads] [10 runs] : 6744950</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[8 threads] [10 runs] : 7247691</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[16 threads] [10 runs] : 7510042</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[32 threads] [10 runs] : 7652880</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[64 threads] [10 runs] : 7761247</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[128 threads] [10 runs] : 7898865</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_10k_s100.txt],[256 threads] [10 runs] : 8099464</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[1 threads] [10 runs] : 94980151</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[2 threads] [10 runs] : 145729235</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[4 threads] [10 runs] : 171183845</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[8 threads] [10 runs] : 183907075</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[16 threads] [10 runs] : 190297346</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[32 threads] [10 runs] : 193559411</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[64 threads] [10 runs] : 195674904</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[128 threads] [10 runs] : 197357545</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_50k_s200.txt],[256 threads] [10 runs] : 198676834</t>
+  </si>
+  <si>
+    <t>[openMP Parallel] , [input_100k_s300.txt],[1 threads] [10 runs] : 372187615</t>
+  </si>
+  <si>
+    <t>[STL</t>
+  </si>
+  <si>
+    <t>CPP</t>
+  </si>
+  <si>
+    <t>Parallel]</t>
+  </si>
+  <si>
+    <t>[input_10k_s100.txt]</t>
+  </si>
+  <si>
+    <t>[1</t>
+  </si>
+  <si>
+    <t>threads]</t>
+  </si>
+  <si>
+    <t>[10</t>
+  </si>
+  <si>
+    <t>runs]</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>[2</t>
+  </si>
+  <si>
+    <t>[4</t>
+  </si>
+  <si>
+    <t>[8</t>
+  </si>
+  <si>
+    <t>[16</t>
+  </si>
+  <si>
+    <t>[32</t>
+  </si>
+  <si>
+    <t>[64</t>
+  </si>
+  <si>
+    <t>[128</t>
+  </si>
+  <si>
+    <t>[256</t>
+  </si>
+  <si>
+    <t>[input_50k_s200.txt]</t>
+  </si>
+  <si>
+    <t>[input_100k_s300.txt]</t>
   </si>
 </sst>
 </file>
@@ -4293,6 +4501,840 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'STL Par'!$J$1:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3776222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5769884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6771237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7289624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7588830</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7815029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7958853</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8095927</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8233801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A53-8C48-918A-C04FE7F43BF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1055768192"/>
+        <c:axId val="1055769840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1055768192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1055769840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1055769840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1055768192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'STL Par'!$J$11:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>95822291</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145906655</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171031920</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>183662821</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>190175093</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>193723379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196010002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>197739857</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199259843</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A658-6E45-AED4-16B31F01A556}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1053765712"/>
+        <c:axId val="1053436960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1053765712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1053436960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1053436960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1053765712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'STL Par'!$J$21:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>373559613</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>570781578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>669413589</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>718979442</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>744112360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>757097875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>765196324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>770888040</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>776237635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BEC-7645-B9FE-84E636DCDE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1056080016"/>
+        <c:axId val="1056070096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1056080016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1056070096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1056070096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1056080016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4414,6 +5456,126 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6517,6 +7679,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6668,6 +9378,119 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E8C971-9180-BC49-BC7E-6AC871F2A33B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2FA9CFE-D210-BC4A-9187-EA58D78FEB85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26D1597B-DD5D-A24A-8451-B47595F499CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -22972,7 +25795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961C2C5D-813E-A846-965D-2AF7B9FA2674}">
   <dimension ref="A1:G258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:F12"/>
     </sheetView>
   </sheetViews>
@@ -26158,4 +28981,1214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016BF22C-B95C-5840-B0AB-93C3BCF9173D}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10F8F44-F033-274A-BB85-24E73ED556AB}">
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I1" t="s">
+        <v>324</v>
+      </c>
+      <c r="J1">
+        <v>3776222</v>
+      </c>
+      <c r="K1">
+        <f>J1/3776222</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2">
+        <v>5769884</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K9" si="0">J2/3776222</f>
+        <v>1.5279514816660673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H3" t="s">
+        <v>323</v>
+      </c>
+      <c r="I3" t="s">
+        <v>324</v>
+      </c>
+      <c r="J3">
+        <v>6771237</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>1.7931247156549588</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H4" t="s">
+        <v>323</v>
+      </c>
+      <c r="I4" t="s">
+        <v>324</v>
+      </c>
+      <c r="J4">
+        <v>7289624</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>1.9304013376332219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5" t="s">
+        <v>328</v>
+      </c>
+      <c r="F5" t="s">
+        <v>321</v>
+      </c>
+      <c r="G5" t="s">
+        <v>322</v>
+      </c>
+      <c r="H5" t="s">
+        <v>323</v>
+      </c>
+      <c r="I5" t="s">
+        <v>324</v>
+      </c>
+      <c r="J5">
+        <v>7588830</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>2.0096355563841319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G6" t="s">
+        <v>322</v>
+      </c>
+      <c r="H6" t="s">
+        <v>323</v>
+      </c>
+      <c r="I6" t="s">
+        <v>324</v>
+      </c>
+      <c r="J6">
+        <v>7815029</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>2.0695364308560249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" t="s">
+        <v>330</v>
+      </c>
+      <c r="F7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G7" t="s">
+        <v>322</v>
+      </c>
+      <c r="H7" t="s">
+        <v>323</v>
+      </c>
+      <c r="I7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J7">
+        <v>7958853</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>2.1076231746968266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8" t="s">
+        <v>331</v>
+      </c>
+      <c r="F8" t="s">
+        <v>321</v>
+      </c>
+      <c r="G8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H8" t="s">
+        <v>323</v>
+      </c>
+      <c r="I8" t="s">
+        <v>324</v>
+      </c>
+      <c r="J8">
+        <v>8095927</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>2.143922417696841</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>316</v>
+      </c>
+      <c r="B9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E9" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" t="s">
+        <v>321</v>
+      </c>
+      <c r="G9" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I9" t="s">
+        <v>324</v>
+      </c>
+      <c r="J9">
+        <v>8233801</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>2.1804335126483561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F11" t="s">
+        <v>321</v>
+      </c>
+      <c r="G11" t="s">
+        <v>322</v>
+      </c>
+      <c r="H11" t="s">
+        <v>323</v>
+      </c>
+      <c r="I11" t="s">
+        <v>324</v>
+      </c>
+      <c r="J11">
+        <v>95822291</v>
+      </c>
+      <c r="K11">
+        <f>J11/95822291</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>316</v>
+      </c>
+      <c r="B12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H12" t="s">
+        <v>323</v>
+      </c>
+      <c r="I12" t="s">
+        <v>324</v>
+      </c>
+      <c r="J12">
+        <v>145906655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" t="s">
+        <v>317</v>
+      </c>
+      <c r="C13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" t="s">
+        <v>326</v>
+      </c>
+      <c r="F13" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" t="s">
+        <v>322</v>
+      </c>
+      <c r="H13" t="s">
+        <v>323</v>
+      </c>
+      <c r="I13" t="s">
+        <v>324</v>
+      </c>
+      <c r="J13">
+        <v>171031920</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" t="s">
+        <v>333</v>
+      </c>
+      <c r="E14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" t="s">
+        <v>321</v>
+      </c>
+      <c r="G14" t="s">
+        <v>322</v>
+      </c>
+      <c r="H14" t="s">
+        <v>323</v>
+      </c>
+      <c r="I14" t="s">
+        <v>324</v>
+      </c>
+      <c r="J14">
+        <v>183662821</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15" t="s">
+        <v>333</v>
+      </c>
+      <c r="E15" t="s">
+        <v>328</v>
+      </c>
+      <c r="F15" t="s">
+        <v>321</v>
+      </c>
+      <c r="G15" t="s">
+        <v>322</v>
+      </c>
+      <c r="H15" t="s">
+        <v>323</v>
+      </c>
+      <c r="I15" t="s">
+        <v>324</v>
+      </c>
+      <c r="J15">
+        <v>190175093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" t="s">
+        <v>329</v>
+      </c>
+      <c r="F16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G16" t="s">
+        <v>322</v>
+      </c>
+      <c r="H16" t="s">
+        <v>323</v>
+      </c>
+      <c r="I16" t="s">
+        <v>324</v>
+      </c>
+      <c r="J16">
+        <v>193723379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>316</v>
+      </c>
+      <c r="B17" t="s">
+        <v>317</v>
+      </c>
+      <c r="C17" t="s">
+        <v>318</v>
+      </c>
+      <c r="D17" t="s">
+        <v>333</v>
+      </c>
+      <c r="E17" t="s">
+        <v>330</v>
+      </c>
+      <c r="F17" t="s">
+        <v>321</v>
+      </c>
+      <c r="G17" t="s">
+        <v>322</v>
+      </c>
+      <c r="H17" t="s">
+        <v>323</v>
+      </c>
+      <c r="I17" t="s">
+        <v>324</v>
+      </c>
+      <c r="J17">
+        <v>196010002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" t="s">
+        <v>317</v>
+      </c>
+      <c r="C18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D18" t="s">
+        <v>333</v>
+      </c>
+      <c r="E18" t="s">
+        <v>331</v>
+      </c>
+      <c r="F18" t="s">
+        <v>321</v>
+      </c>
+      <c r="G18" t="s">
+        <v>322</v>
+      </c>
+      <c r="H18" t="s">
+        <v>323</v>
+      </c>
+      <c r="I18" t="s">
+        <v>324</v>
+      </c>
+      <c r="J18">
+        <v>197739857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" t="s">
+        <v>318</v>
+      </c>
+      <c r="D19" t="s">
+        <v>333</v>
+      </c>
+      <c r="E19" t="s">
+        <v>332</v>
+      </c>
+      <c r="F19" t="s">
+        <v>321</v>
+      </c>
+      <c r="G19" t="s">
+        <v>322</v>
+      </c>
+      <c r="H19" t="s">
+        <v>323</v>
+      </c>
+      <c r="I19" t="s">
+        <v>324</v>
+      </c>
+      <c r="J19">
+        <v>199259843</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C21" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" t="s">
+        <v>334</v>
+      </c>
+      <c r="E21" t="s">
+        <v>320</v>
+      </c>
+      <c r="F21" t="s">
+        <v>321</v>
+      </c>
+      <c r="G21" t="s">
+        <v>322</v>
+      </c>
+      <c r="H21" t="s">
+        <v>323</v>
+      </c>
+      <c r="I21" t="s">
+        <v>324</v>
+      </c>
+      <c r="J21">
+        <v>373559613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22" t="s">
+        <v>334</v>
+      </c>
+      <c r="E22" t="s">
+        <v>325</v>
+      </c>
+      <c r="F22" t="s">
+        <v>321</v>
+      </c>
+      <c r="G22" t="s">
+        <v>322</v>
+      </c>
+      <c r="H22" t="s">
+        <v>323</v>
+      </c>
+      <c r="I22" t="s">
+        <v>324</v>
+      </c>
+      <c r="J22">
+        <v>570781578</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B23" t="s">
+        <v>317</v>
+      </c>
+      <c r="C23" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" t="s">
+        <v>326</v>
+      </c>
+      <c r="F23" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" t="s">
+        <v>322</v>
+      </c>
+      <c r="H23" t="s">
+        <v>323</v>
+      </c>
+      <c r="I23" t="s">
+        <v>324</v>
+      </c>
+      <c r="J23">
+        <v>669413589</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E24" t="s">
+        <v>327</v>
+      </c>
+      <c r="F24" t="s">
+        <v>321</v>
+      </c>
+      <c r="G24" t="s">
+        <v>322</v>
+      </c>
+      <c r="H24" t="s">
+        <v>323</v>
+      </c>
+      <c r="I24" t="s">
+        <v>324</v>
+      </c>
+      <c r="J24">
+        <v>718979442</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>316</v>
+      </c>
+      <c r="B25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" t="s">
+        <v>334</v>
+      </c>
+      <c r="E25" t="s">
+        <v>328</v>
+      </c>
+      <c r="F25" t="s">
+        <v>321</v>
+      </c>
+      <c r="G25" t="s">
+        <v>322</v>
+      </c>
+      <c r="H25" t="s">
+        <v>323</v>
+      </c>
+      <c r="I25" t="s">
+        <v>324</v>
+      </c>
+      <c r="J25">
+        <v>744112360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26" t="s">
+        <v>334</v>
+      </c>
+      <c r="E26" t="s">
+        <v>329</v>
+      </c>
+      <c r="F26" t="s">
+        <v>321</v>
+      </c>
+      <c r="G26" t="s">
+        <v>322</v>
+      </c>
+      <c r="H26" t="s">
+        <v>323</v>
+      </c>
+      <c r="I26" t="s">
+        <v>324</v>
+      </c>
+      <c r="J26">
+        <v>757097875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>316</v>
+      </c>
+      <c r="B27" t="s">
+        <v>317</v>
+      </c>
+      <c r="C27" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" t="s">
+        <v>330</v>
+      </c>
+      <c r="F27" t="s">
+        <v>321</v>
+      </c>
+      <c r="G27" t="s">
+        <v>322</v>
+      </c>
+      <c r="H27" t="s">
+        <v>323</v>
+      </c>
+      <c r="I27" t="s">
+        <v>324</v>
+      </c>
+      <c r="J27">
+        <v>765196324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>316</v>
+      </c>
+      <c r="B28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" t="s">
+        <v>334</v>
+      </c>
+      <c r="E28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F28" t="s">
+        <v>321</v>
+      </c>
+      <c r="G28" t="s">
+        <v>322</v>
+      </c>
+      <c r="H28" t="s">
+        <v>323</v>
+      </c>
+      <c r="I28" t="s">
+        <v>324</v>
+      </c>
+      <c r="J28">
+        <v>770888040</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>316</v>
+      </c>
+      <c r="B29" t="s">
+        <v>317</v>
+      </c>
+      <c r="C29" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29" t="s">
+        <v>334</v>
+      </c>
+      <c r="E29" t="s">
+        <v>332</v>
+      </c>
+      <c r="F29" t="s">
+        <v>321</v>
+      </c>
+      <c r="G29" t="s">
+        <v>322</v>
+      </c>
+      <c r="H29" t="s">
+        <v>323</v>
+      </c>
+      <c r="I29" t="s">
+        <v>324</v>
+      </c>
+      <c r="J29">
+        <v>776237635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB0B69E-7658-9B4C-B675-43270FB90A7F}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E6B775-C6FB-A74E-8D73-7CE27EDED807}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>